<commit_message>
added two-stage delay to ReleaseFrisbeeCommand: after opening, after closing
</commit_message>
<xml_diff>
--- a/new_shooter_data.xlsx
+++ b/new_shooter_data.xlsx
@@ -4,15 +4,36 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="cal_1" localSheetId="1">Sheet2!$A$1:$B$45</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="cal" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\irving\Desktop\cal.txt" space="1" consecutive="1" delimiter=":">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -89,7 +110,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -173,7 +193,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>257.7</c:v>
+                  <c:v>719.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>606</c:v>
@@ -224,11 +244,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51137152"/>
-        <c:axId val="51135616"/>
+        <c:axId val="121635968"/>
+        <c:axId val="121637504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51137152"/>
+        <c:axId val="121635968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -238,12 +258,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51135616"/>
+        <c:crossAx val="121637504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51135616"/>
+        <c:axId val="121637504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -254,14 +274,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51137152"/>
+        <c:crossAx val="121635968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -291,7 +310,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -316,7 +334,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="#,##0.00000000000000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -390,11 +407,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115050752"/>
-        <c:axId val="115049216"/>
+        <c:axId val="121666944"/>
+        <c:axId val="121676928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115050752"/>
+        <c:axId val="121666944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,12 +421,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115049216"/>
+        <c:crossAx val="121676928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115049216"/>
+        <c:axId val="121676928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,7 +437,274 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115050752"/>
+        <c:crossAx val="121666944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>RPM-Power</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="#,##0.000000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B:$B</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>1968.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1968.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1968.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2229.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2229.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2229.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2656.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2656.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2656.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2852.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2852.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2852.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2998.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2998.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2998.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3111.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3111.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3111.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3304.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3304.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3304.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3519.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3519.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3519.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$A:$A</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="121612928"/>
+        <c:axId val="121618816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="121612928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121618816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="121618816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121612928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -505,6 +789,45 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cal_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -796,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +1146,7 @@
         <v>0.25</v>
       </c>
       <c r="B3">
-        <v>257.7</v>
+        <v>719.6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,13 +1259,218 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.5</v>
+      </c>
+      <c r="B1">
+        <v>1968.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>1968.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>1968.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B4">
+        <v>2229.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B5">
+        <v>2229.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B6">
+        <v>2229.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.65</v>
+      </c>
+      <c r="B7">
+        <v>2656.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.65</v>
+      </c>
+      <c r="B8">
+        <v>2656.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.65</v>
+      </c>
+      <c r="B9">
+        <v>2656.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.7</v>
+      </c>
+      <c r="B10">
+        <v>2852.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>2852.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.7</v>
+      </c>
+      <c r="B12">
+        <v>2852.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.75</v>
+      </c>
+      <c r="B13">
+        <v>2998.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.75</v>
+      </c>
+      <c r="B14">
+        <v>2998.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.75</v>
+      </c>
+      <c r="B15">
+        <v>2998.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.8</v>
+      </c>
+      <c r="B16">
+        <v>3111.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.8</v>
+      </c>
+      <c r="B17">
+        <v>3111.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.8</v>
+      </c>
+      <c r="B18">
+        <v>3111.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.85</v>
+      </c>
+      <c r="B19">
+        <v>3304.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.85</v>
+      </c>
+      <c r="B20">
+        <v>3304.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.85</v>
+      </c>
+      <c r="B21">
+        <v>3304.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.9</v>
+      </c>
+      <c r="B22">
+        <v>3519.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.9</v>
+      </c>
+      <c r="B23">
+        <v>3519.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.9</v>
+      </c>
+      <c r="B24">
+        <v>3519.7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>